<commit_message>
adds the first functioning score-computation pipeline
</commit_message>
<xml_diff>
--- a/data/PLACEHOLDER-country-features-vs-surveillance-approaches.xlsx
+++ b/data/PLACEHOLDER-country-features-vs-surveillance-approaches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/EIOSCoreTeamIII/Shared Documents/Data Science for PHI/SPA-data-science/SPA-algorithm-demo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/EIOSCoreTeamIII/Shared Documents/Data Science for PHI/SPA-data-science/SPA.Algorithm.Demo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD0ACABB-9626-4389-910E-6525B24C2D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{DD0ACABB-9626-4389-910E-6525B24C2D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF9FEB27-0424-4AE0-BA5D-03C7D3996EE2}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{5A4A515B-250C-4D32-ACBA-E4989C42686A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A4A515B-250C-4D32-ACBA-E4989C42686A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>Climate monitoring</t>
   </si>
   <si>
-    <t>Country feature</t>
-  </si>
-  <si>
     <t>Natural</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Context type</t>
   </si>
 </sst>
 </file>
@@ -204,14 +204,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -558,7 +558,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A5" sqref="A5"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +568,7 @@
   <sheetData>
     <row r="1" spans="1:28" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -654,13 +654,13 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6">
         <v>0</v>
@@ -699,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="6">
         <v>0</v>
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T2" s="6">
         <v>0</v>
@@ -717,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W2" s="6">
         <v>0</v>
@@ -735,21 +735,21 @@
         <v>0</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="6">
         <v>0</v>
@@ -773,7 +773,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M3" s="6">
         <v>0</v>
@@ -785,34 +785,34 @@
         <v>0</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="6">
         <v>0</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T3" s="6">
         <v>0</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V3" s="6">
         <v>0</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z3" s="6">
         <v>0</v>
@@ -821,12 +821,12 @@
         <v>0</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="6">
         <v>0</v>
@@ -835,76 +835,76 @@
         <v>0</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R4" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6">
+        <v>0</v>
+      </c>
+      <c r="U4" s="6">
+        <v>0</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0</v>
+      </c>
+      <c r="W4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="X4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-      <c r="O4" s="6">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="R4" s="6">
-        <v>0</v>
-      </c>
-      <c r="S4" s="6">
-        <v>0</v>
-      </c>
-      <c r="T4" s="6">
-        <v>0</v>
-      </c>
-      <c r="U4" s="6">
-        <v>0</v>
-      </c>
-      <c r="V4" s="6">
-        <v>0</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="Y4" s="6">
         <v>0</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB4" s="6">
         <v>0</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="5" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="6">
         <v>0</v>
@@ -927,70 +927,70 @@
         <v>0</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+      <c r="R5" s="6">
+        <v>0</v>
+      </c>
+      <c r="S5" s="6">
+        <v>0</v>
+      </c>
+      <c r="T5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="U5" s="6">
+        <v>0</v>
+      </c>
+      <c r="V5" s="6">
+        <v>0</v>
+      </c>
+      <c r="W5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="X5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>0</v>
-      </c>
-      <c r="R5" s="6">
-        <v>0</v>
-      </c>
-      <c r="S5" s="6">
-        <v>0</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U5" s="6">
-        <v>0</v>
-      </c>
-      <c r="V5" s="6">
-        <v>0</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="Y5" s="6">
         <v>0</v>
       </c>
       <c r="Z5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB5" s="6">
         <v>0</v>
@@ -1278,15 +1278,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="97eadeb2-cd7a-457f-ac14-0ed0556ce061">
@@ -1299,14 +1290,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{198BC500-993A-4742-A558-DBAF535C6D71}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{198BC500-993A-4742-A558-DBAF535C6D71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="97eadeb2-cd7a-457f-ac14-0ed0556ce061"/>
+    <ds:schemaRef ds:uri="97c8a684-1c4b-4244-9323-fa8d251df7dc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59DB8049-913B-456E-A74B-631B77F9AE40}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DEAE421-F23A-4419-8944-B2719B12189D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="97eadeb2-cd7a-457f-ac14-0ed0556ce061"/>
+    <ds:schemaRef ds:uri="97c8a684-1c4b-4244-9323-fa8d251df7dc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DEAE421-F23A-4419-8944-B2719B12189D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59DB8049-913B-456E-A74B-631B77F9AE40}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>